<commit_message>
added notes from the meeting today with SOM
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Takano_fellowship/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8077FF73-FB40-E64C-9AF6-F387EBA89975}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E94C05-38BD-3743-AC30-A93459F4ED83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3500" yWindow="560" windowWidth="25300" windowHeight="16020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4637,7 +4637,7 @@
   <dimension ref="A1:AU37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C7:C8"/>
+      <selection activeCell="A2" sqref="A2:R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4700,56 +4700,56 @@
       <c r="A2" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B2">
-        <v>-600</v>
-      </c>
-      <c r="C2" t="s">
-        <v>74</v>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>133</v>
       </c>
       <c r="D2" s="12">
-        <v>50074</v>
+        <v>1199</v>
       </c>
       <c r="E2" s="12">
-        <v>46974</v>
+        <v>1095</v>
       </c>
       <c r="F2" s="13">
-        <v>0.93810000000000004</v>
-      </c>
-      <c r="G2" s="12">
-        <v>3100</v>
+        <v>0.9133</v>
+      </c>
+      <c r="G2">
+        <v>104</v>
       </c>
       <c r="H2" s="13">
-        <v>6.1899999999999997E-2</v>
-      </c>
-      <c r="I2" s="12">
-        <v>41279</v>
-      </c>
-      <c r="J2" s="12">
-        <v>2430</v>
-      </c>
-      <c r="K2" s="12">
-        <v>3265</v>
-      </c>
-      <c r="L2" s="12">
-        <v>1948</v>
+        <v>8.6699999999999999E-2</v>
+      </c>
+      <c r="I2">
+        <v>940</v>
+      </c>
+      <c r="J2">
+        <v>67</v>
+      </c>
+      <c r="K2">
+        <v>88</v>
+      </c>
+      <c r="L2">
+        <v>82</v>
       </c>
       <c r="M2">
-        <v>604</v>
+        <v>17</v>
       </c>
       <c r="N2">
-        <v>247</v>
+        <v>2</v>
       </c>
       <c r="O2">
-        <v>301</v>
+        <v>3</v>
       </c>
       <c r="P2">
-        <v>7.26</v>
+        <v>5.56</v>
       </c>
       <c r="Q2">
-        <v>9.7100000000000009</v>
+        <v>5.68</v>
       </c>
       <c r="R2">
-        <v>4.08</v>
+        <v>12.11</v>
       </c>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
@@ -4757,55 +4757,55 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>133</v>
+        <v>125</v>
+      </c>
+      <c r="C3" t="s">
+        <v>126</v>
       </c>
       <c r="D3" s="12">
-        <v>1199</v>
-      </c>
-      <c r="E3" s="12">
-        <v>1095</v>
+        <v>1047</v>
+      </c>
+      <c r="E3">
+        <v>946</v>
       </c>
       <c r="F3" s="13">
-        <v>0.9133</v>
+        <v>0.90349999999999997</v>
       </c>
       <c r="G3">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H3" s="13">
-        <v>8.6699999999999999E-2</v>
+        <v>9.6500000000000002E-2</v>
       </c>
       <c r="I3">
-        <v>940</v>
+        <v>786</v>
       </c>
       <c r="J3">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K3">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="L3">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="M3">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="N3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P3">
-        <v>5.56</v>
+        <v>10.11</v>
       </c>
       <c r="Q3">
-        <v>5.68</v>
+        <v>11.31</v>
       </c>
       <c r="R3">
-        <v>12.11</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.2">
@@ -4813,55 +4813,55 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="D4" s="12">
-        <v>3105</v>
+        <v>3799</v>
       </c>
       <c r="E4" s="12">
-        <v>2949</v>
+        <v>3748</v>
       </c>
       <c r="F4" s="13">
-        <v>0.94979999999999998</v>
+        <v>0.98660000000000003</v>
       </c>
       <c r="G4">
-        <v>156</v>
+        <v>51</v>
       </c>
       <c r="H4" s="13">
-        <v>5.0200000000000002E-2</v>
+        <v>1.34E-2</v>
       </c>
       <c r="I4" s="12">
-        <v>2585</v>
+        <v>3292</v>
       </c>
       <c r="J4">
-        <v>153</v>
+        <v>290</v>
       </c>
       <c r="K4">
-        <v>211</v>
+        <v>166</v>
       </c>
       <c r="L4">
-        <v>125</v>
+        <v>33</v>
       </c>
       <c r="M4">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="N4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O4">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="P4">
-        <v>7.55</v>
+        <v>3.58</v>
       </c>
       <c r="Q4">
-        <v>10.36</v>
+        <v>3.27</v>
       </c>
       <c r="R4">
-        <v>4.87</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.2">
@@ -4869,40 +4869,40 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="12">
-        <v>1275</v>
-      </c>
-      <c r="E5" s="12">
-        <v>1271</v>
+        <v>97</v>
+      </c>
+      <c r="D5">
+        <v>48</v>
+      </c>
+      <c r="E5">
+        <v>48</v>
       </c>
       <c r="F5" s="13">
-        <v>0.99690000000000001</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H5" s="13">
-        <v>3.0999999999999999E-3</v>
-      </c>
-      <c r="I5" s="12">
-        <v>1254</v>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>44</v>
       </c>
       <c r="J5">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="K5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -4911,10 +4911,13 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>5.35</v>
+        <v>1.96</v>
       </c>
       <c r="Q5">
-        <v>1.76</v>
+        <v>4.5</v>
+      </c>
+      <c r="R5">
+        <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.2">
@@ -4922,40 +4925,40 @@
         <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" s="12">
-        <v>1218</v>
+        <v>1275</v>
       </c>
       <c r="E6" s="12">
-        <v>1199</v>
+        <v>1271</v>
       </c>
       <c r="F6" s="13">
-        <v>0.98440000000000005</v>
+        <v>0.99690000000000001</v>
       </c>
       <c r="G6">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="H6" s="13">
-        <v>1.5599999999999999E-2</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="I6" s="12">
-        <v>1052</v>
+        <v>1254</v>
       </c>
       <c r="J6">
-        <v>96</v>
+        <v>13</v>
       </c>
       <c r="K6">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="L6">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -4964,13 +4967,10 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>4.12</v>
+        <v>5.35</v>
       </c>
       <c r="Q6">
-        <v>12.92</v>
-      </c>
-      <c r="R6">
-        <v>2.61</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="7" spans="1:47" x14ac:dyDescent="0.2">
@@ -4978,40 +4978,40 @@
         <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="D7" s="12">
-        <v>1519</v>
+        <v>2116</v>
       </c>
       <c r="E7" s="12">
-        <v>1464</v>
+        <v>2081</v>
       </c>
       <c r="F7" s="13">
-        <v>0.96379999999999999</v>
+        <v>0.98350000000000004</v>
       </c>
       <c r="G7">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="H7" s="13">
-        <v>3.6200000000000003E-2</v>
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="I7" s="12">
-        <v>1220</v>
+        <v>1944</v>
       </c>
       <c r="J7">
-        <v>157</v>
+        <v>73</v>
       </c>
       <c r="K7">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="L7">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="M7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -5020,125 +5020,125 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>5.76</v>
+        <v>0.76</v>
       </c>
       <c r="Q7">
-        <v>10.62</v>
+        <v>2.78</v>
       </c>
       <c r="R7">
-        <v>4.28</v>
+        <v>5.27</v>
       </c>
     </row>
     <row r="8" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B8">
-        <v>-605</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="D8" s="12">
-        <v>53000</v>
-      </c>
-      <c r="E8" s="12">
-        <v>49794</v>
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8">
+        <v>842</v>
+      </c>
+      <c r="E8">
+        <v>822</v>
       </c>
       <c r="F8" s="13">
-        <v>0.9395</v>
-      </c>
-      <c r="G8" s="12">
-        <v>3206</v>
+        <v>0.97619999999999996</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
       </c>
       <c r="H8" s="13">
-        <v>6.0499999999999998E-2</v>
-      </c>
-      <c r="I8" s="12">
-        <v>43104</v>
-      </c>
-      <c r="J8" s="12">
-        <v>2813</v>
-      </c>
-      <c r="K8" s="12">
-        <v>3877</v>
-      </c>
-      <c r="L8" s="12">
-        <v>2353</v>
+        <v>2.3800000000000002E-2</v>
+      </c>
+      <c r="I8">
+        <v>737</v>
+      </c>
+      <c r="J8">
+        <v>38</v>
+      </c>
+      <c r="K8">
+        <v>47</v>
+      </c>
+      <c r="L8">
+        <v>20</v>
       </c>
       <c r="M8">
-        <v>532</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>207</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="P8">
-        <v>3.22</v>
+        <v>0.43</v>
       </c>
       <c r="Q8">
-        <v>8.91</v>
+        <v>2</v>
       </c>
       <c r="R8">
-        <v>4.74</v>
+        <v>9.09</v>
       </c>
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B9">
-        <v>-605</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="D9" s="12">
-        <v>23425</v>
-      </c>
-      <c r="E9" s="12">
-        <v>21621</v>
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9">
+        <v>955</v>
+      </c>
+      <c r="E9">
+        <v>944</v>
       </c>
       <c r="F9" s="13">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="G9" s="12">
-        <v>1804</v>
+        <v>0.98850000000000005</v>
+      </c>
+      <c r="G9">
+        <v>11</v>
       </c>
       <c r="H9" s="13">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="I9" s="12">
-        <v>18397</v>
-      </c>
-      <c r="J9" s="12">
-        <v>1369</v>
-      </c>
-      <c r="K9" s="12">
-        <v>1855</v>
-      </c>
-      <c r="L9" s="12">
-        <v>1250</v>
+        <v>1.15E-2</v>
+      </c>
+      <c r="I9">
+        <v>929</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>12</v>
+      </c>
+      <c r="L9">
+        <v>9</v>
       </c>
       <c r="M9">
-        <v>347</v>
+        <v>2</v>
       </c>
       <c r="N9">
-        <v>146</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>2.33</v>
+        <v>0.64</v>
       </c>
       <c r="Q9">
-        <v>8.77</v>
+        <v>15</v>
       </c>
       <c r="R9">
-        <v>2.2599999999999998</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="10" spans="1:47" x14ac:dyDescent="0.2">
@@ -5146,55 +5146,55 @@
         <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="D10" s="12">
-        <v>20457</v>
+        <v>1515</v>
       </c>
       <c r="E10" s="12">
-        <v>19210</v>
+        <v>1506</v>
       </c>
       <c r="F10" s="13">
-        <v>0.93899999999999995</v>
-      </c>
-      <c r="G10" s="12">
-        <v>1247</v>
+        <v>0.99409999999999998</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
       </c>
       <c r="H10" s="13">
-        <v>6.0999999999999999E-2</v>
+        <v>5.8999999999999999E-3</v>
       </c>
       <c r="I10" s="12">
-        <v>16493</v>
-      </c>
-      <c r="J10" s="12">
-        <v>1088</v>
-      </c>
-      <c r="K10" s="12">
-        <v>1629</v>
+        <v>1430</v>
+      </c>
+      <c r="J10">
+        <v>41</v>
+      </c>
+      <c r="K10">
+        <v>35</v>
       </c>
       <c r="L10">
-        <v>977</v>
+        <v>9</v>
       </c>
       <c r="M10">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>4.17</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="Q10">
-        <v>9.8699999999999992</v>
+        <v>10.6</v>
       </c>
       <c r="R10">
-        <v>4.3099999999999996</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="11" spans="1:47" x14ac:dyDescent="0.2">
@@ -5202,111 +5202,111 @@
         <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="12">
-        <v>1582</v>
-      </c>
-      <c r="E11" s="12">
-        <v>1558</v>
+        <v>118</v>
+      </c>
+      <c r="D11">
+        <v>716</v>
+      </c>
+      <c r="E11">
+        <v>716</v>
       </c>
       <c r="F11" s="13">
-        <v>0.98480000000000001</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="H11" s="13">
-        <v>1.52E-2</v>
-      </c>
-      <c r="I11" s="12">
-        <v>1415</v>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>709</v>
       </c>
       <c r="J11">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="K11">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="L11">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N11">
         <v>0</v>
       </c>
       <c r="O11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>0.51</v>
+        <v>0.31</v>
       </c>
       <c r="Q11">
-        <v>4</v>
+        <v>0.06</v>
       </c>
       <c r="R11">
-        <v>6.16</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" t="s">
         <v>73</v>
       </c>
-      <c r="B12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" t="s">
-        <v>89</v>
+      <c r="B12">
+        <v>-691</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>137</v>
       </c>
       <c r="D12" s="12">
-        <v>2251</v>
+        <v>66418</v>
       </c>
       <c r="E12" s="12">
-        <v>2220</v>
+        <v>62380</v>
       </c>
       <c r="F12" s="13">
-        <v>0.98619999999999997</v>
-      </c>
-      <c r="G12">
-        <v>31</v>
+        <v>0.93920000000000003</v>
+      </c>
+      <c r="G12" s="12">
+        <v>4038</v>
       </c>
       <c r="H12" s="13">
-        <v>1.38E-2</v>
+        <v>6.08E-2</v>
       </c>
       <c r="I12" s="12">
-        <v>2054</v>
-      </c>
-      <c r="J12">
-        <v>83</v>
-      </c>
-      <c r="K12">
-        <v>83</v>
-      </c>
-      <c r="L12">
-        <v>22</v>
+        <v>54042</v>
+      </c>
+      <c r="J12" s="12">
+        <v>3717</v>
+      </c>
+      <c r="K12" s="12">
+        <v>4621</v>
+      </c>
+      <c r="L12" s="12">
+        <v>3141</v>
       </c>
       <c r="M12">
-        <v>5</v>
+        <v>605</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>181</v>
       </c>
       <c r="O12">
-        <v>4</v>
+        <v>111</v>
       </c>
       <c r="P12">
-        <v>2.13</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="Q12">
-        <v>5.58</v>
+        <v>8.7200000000000006</v>
       </c>
       <c r="R12">
-        <v>5.77</v>
+        <v>4.6900000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:47" x14ac:dyDescent="0.2">
@@ -5314,55 +5314,55 @@
         <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="12">
-        <v>2464</v>
-      </c>
-      <c r="E13" s="12">
-        <v>2453</v>
+        <v>103</v>
+      </c>
+      <c r="D13">
+        <v>562</v>
+      </c>
+      <c r="E13">
+        <v>553</v>
       </c>
       <c r="F13" s="13">
-        <v>0.99550000000000005</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="G13">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H13" s="13">
-        <v>4.4999999999999997E-3</v>
-      </c>
-      <c r="I13" s="12">
-        <v>2337</v>
+        <v>1.6E-2</v>
+      </c>
+      <c r="I13">
+        <v>495</v>
       </c>
       <c r="J13">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="K13">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="L13">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13">
         <v>0</v>
       </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>2</v>
-      </c>
       <c r="P13">
-        <v>1.25</v>
+        <v>1.79</v>
       </c>
       <c r="Q13">
-        <v>2.1800000000000002</v>
+        <v>11.05</v>
       </c>
       <c r="R13">
-        <v>2.16</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.2">
@@ -5370,40 +5370,40 @@
         <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14">
-        <v>842</v>
-      </c>
-      <c r="E14">
-        <v>822</v>
+        <v>83</v>
+      </c>
+      <c r="D14" s="12">
+        <v>1519</v>
+      </c>
+      <c r="E14" s="12">
+        <v>1464</v>
       </c>
       <c r="F14" s="13">
-        <v>0.97619999999999996</v>
+        <v>0.96379999999999999</v>
       </c>
       <c r="G14">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="H14" s="13">
-        <v>2.3800000000000002E-2</v>
-      </c>
-      <c r="I14">
-        <v>737</v>
+        <v>3.6200000000000003E-2</v>
+      </c>
+      <c r="I14" s="12">
+        <v>1220</v>
       </c>
       <c r="J14">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="K14">
+        <v>87</v>
+      </c>
+      <c r="L14">
         <v>47</v>
       </c>
-      <c r="L14">
-        <v>20</v>
-      </c>
       <c r="M14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -5412,13 +5412,13 @@
         <v>0</v>
       </c>
       <c r="P14">
-        <v>0.43</v>
+        <v>5.76</v>
       </c>
       <c r="Q14">
-        <v>2</v>
+        <v>10.62</v>
       </c>
       <c r="R14">
-        <v>9.09</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.2">
@@ -5426,111 +5426,111 @@
         <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D15" s="12">
-        <v>1931</v>
+        <v>20457</v>
       </c>
       <c r="E15" s="12">
-        <v>1862</v>
+        <v>19210</v>
       </c>
       <c r="F15" s="13">
-        <v>0.96430000000000005</v>
-      </c>
-      <c r="G15">
-        <v>69</v>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="G15" s="12">
+        <v>1247</v>
       </c>
       <c r="H15" s="13">
-        <v>3.5700000000000003E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="I15" s="12">
-        <v>1627</v>
-      </c>
-      <c r="J15">
-        <v>124</v>
-      </c>
-      <c r="K15">
-        <v>111</v>
+        <v>16493</v>
+      </c>
+      <c r="J15" s="12">
+        <v>1088</v>
+      </c>
+      <c r="K15" s="12">
+        <v>1629</v>
       </c>
       <c r="L15">
-        <v>54</v>
+        <v>977</v>
       </c>
       <c r="M15">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="O15">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="P15">
-        <v>5.49</v>
+        <v>4.17</v>
       </c>
       <c r="Q15">
-        <v>6.71</v>
+        <v>9.8699999999999992</v>
       </c>
       <c r="R15">
-        <v>7.21</v>
+        <v>4.3099999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16">
-        <v>48</v>
-      </c>
-      <c r="E16">
-        <v>48</v>
+      <c r="B16">
+        <v>-605</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="12">
+        <v>53000</v>
+      </c>
+      <c r="E16" s="12">
+        <v>49794</v>
       </c>
       <c r="F16" s="13">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
+        <v>0.9395</v>
+      </c>
+      <c r="G16" s="12">
+        <v>3206</v>
       </c>
       <c r="H16" s="13">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>44</v>
-      </c>
-      <c r="J16">
-        <v>2</v>
-      </c>
-      <c r="K16">
-        <v>2</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
+        <v>6.0499999999999998E-2</v>
+      </c>
+      <c r="I16" s="12">
+        <v>43104</v>
+      </c>
+      <c r="J16" s="12">
+        <v>2813</v>
+      </c>
+      <c r="K16" s="12">
+        <v>3877</v>
+      </c>
+      <c r="L16" s="12">
+        <v>2353</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>532</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>207</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="P16">
-        <v>1.96</v>
+        <v>3.22</v>
       </c>
       <c r="Q16">
-        <v>4.5</v>
+        <v>8.91</v>
       </c>
       <c r="R16">
-        <v>1.1100000000000001</v>
+        <v>4.74</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -5538,102 +5538,111 @@
         <v>73</v>
       </c>
       <c r="B17">
-        <v>-664</v>
-      </c>
-      <c r="C17" t="s">
-        <v>98</v>
+        <v>-605</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>135</v>
       </c>
       <c r="D17" s="12">
-        <v>35352</v>
+        <v>23425</v>
       </c>
       <c r="E17" s="12">
-        <v>34542</v>
+        <v>21621</v>
       </c>
       <c r="F17" s="13">
-        <v>0.97709999999999997</v>
-      </c>
-      <c r="G17">
-        <v>810</v>
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="G17" s="12">
+        <v>1804</v>
       </c>
       <c r="H17" s="13">
-        <v>2.29E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="I17" s="12">
-        <v>32679</v>
-      </c>
-      <c r="J17">
-        <v>815</v>
+        <v>18397</v>
+      </c>
+      <c r="J17" s="12">
+        <v>1369</v>
       </c>
       <c r="K17" s="12">
-        <v>1048</v>
-      </c>
-      <c r="L17">
-        <v>557</v>
+        <v>1855</v>
+      </c>
+      <c r="L17" s="12">
+        <v>1250</v>
       </c>
       <c r="M17">
-        <v>184</v>
+        <v>347</v>
       </c>
       <c r="N17">
-        <v>58</v>
+        <v>146</v>
       </c>
       <c r="O17">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="P17">
-        <v>0.63</v>
+        <v>2.33</v>
       </c>
       <c r="Q17">
-        <v>3.84</v>
+        <v>8.77</v>
       </c>
       <c r="R17">
-        <v>1.84</v>
+        <v>2.2599999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B18" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D18">
-        <v>66</v>
-      </c>
-      <c r="E18">
-        <v>66</v>
+      <c r="B18">
+        <v>-600</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="12">
+        <v>50074</v>
+      </c>
+      <c r="E18" s="12">
+        <v>46974</v>
       </c>
       <c r="F18" s="13">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
+        <v>0.93810000000000004</v>
+      </c>
+      <c r="G18" s="12">
+        <v>3100</v>
       </c>
       <c r="H18" s="13">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>66</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
+        <v>6.1899999999999997E-2</v>
+      </c>
+      <c r="I18" s="12">
+        <v>41279</v>
+      </c>
+      <c r="J18" s="12">
+        <v>2430</v>
+      </c>
+      <c r="K18" s="12">
+        <v>3265</v>
+      </c>
+      <c r="L18" s="12">
+        <v>1948</v>
       </c>
       <c r="M18">
-        <v>0</v>
+        <v>604</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>247</v>
       </c>
       <c r="O18">
-        <v>0</v>
+        <v>301</v>
+      </c>
+      <c r="P18">
+        <v>7.26</v>
+      </c>
+      <c r="Q18">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="R18">
+        <v>4.08</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
@@ -5641,55 +5650,55 @@
         <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="D19" s="12">
-        <v>11083</v>
+        <v>8106</v>
       </c>
       <c r="E19" s="12">
-        <v>10868</v>
+        <v>7751</v>
       </c>
       <c r="F19" s="13">
-        <v>0.98060000000000003</v>
+        <v>0.95620000000000005</v>
       </c>
       <c r="G19">
-        <v>215</v>
+        <v>355</v>
       </c>
       <c r="H19" s="13">
-        <v>1.9400000000000001E-2</v>
+        <v>4.3799999999999999E-2</v>
       </c>
       <c r="I19" s="12">
-        <v>9675</v>
+        <v>6947</v>
       </c>
       <c r="J19">
-        <v>447</v>
+        <v>340</v>
       </c>
       <c r="K19">
-        <v>746</v>
+        <v>464</v>
       </c>
       <c r="L19">
-        <v>185</v>
+        <v>305</v>
       </c>
       <c r="M19">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="N19">
         <v>7</v>
       </c>
       <c r="O19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P19">
-        <v>0.94</v>
+        <v>5.21</v>
       </c>
       <c r="Q19">
-        <v>5.78</v>
+        <v>5.04</v>
       </c>
       <c r="R19">
-        <v>5.18</v>
+        <v>7.45</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
@@ -5697,55 +5706,55 @@
         <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20">
-        <v>562</v>
-      </c>
-      <c r="E20">
-        <v>553</v>
+        <v>101</v>
+      </c>
+      <c r="D20" s="12">
+        <v>11083</v>
+      </c>
+      <c r="E20" s="12">
+        <v>10868</v>
       </c>
       <c r="F20" s="13">
-        <v>0.98399999999999999</v>
+        <v>0.98060000000000003</v>
       </c>
       <c r="G20">
-        <v>9</v>
+        <v>215</v>
       </c>
       <c r="H20" s="13">
-        <v>1.6E-2</v>
-      </c>
-      <c r="I20">
-        <v>495</v>
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="I20" s="12">
+        <v>9675</v>
       </c>
       <c r="J20">
-        <v>32</v>
+        <v>447</v>
       </c>
       <c r="K20">
-        <v>26</v>
+        <v>746</v>
       </c>
       <c r="L20">
-        <v>5</v>
+        <v>185</v>
       </c>
       <c r="M20">
+        <v>22</v>
+      </c>
+      <c r="N20">
+        <v>7</v>
+      </c>
+      <c r="O20">
         <v>1</v>
       </c>
-      <c r="N20">
-        <v>3</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
       <c r="P20">
-        <v>1.79</v>
+        <v>0.94</v>
       </c>
       <c r="Q20">
-        <v>11.05</v>
+        <v>5.78</v>
       </c>
       <c r="R20">
-        <v>1.51</v>
+        <v>5.18</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -5753,55 +5762,55 @@
         <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="D21" s="12">
-        <v>8325</v>
+        <v>2251</v>
       </c>
       <c r="E21" s="12">
-        <v>8170</v>
+        <v>2220</v>
       </c>
       <c r="F21" s="13">
-        <v>0.98140000000000005</v>
+        <v>0.98619999999999997</v>
       </c>
       <c r="G21">
-        <v>155</v>
+        <v>31</v>
       </c>
       <c r="H21" s="13">
-        <v>1.8599999999999998E-2</v>
+        <v>1.38E-2</v>
       </c>
       <c r="I21" s="12">
-        <v>7649</v>
+        <v>2054</v>
       </c>
       <c r="J21">
-        <v>233</v>
+        <v>83</v>
       </c>
       <c r="K21">
-        <v>288</v>
+        <v>83</v>
       </c>
       <c r="L21">
-        <v>142</v>
+        <v>22</v>
       </c>
       <c r="M21">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="N21">
         <v>0</v>
       </c>
       <c r="O21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P21">
-        <v>0.73</v>
+        <v>2.13</v>
       </c>
       <c r="Q21">
-        <v>3.51</v>
+        <v>5.58</v>
       </c>
       <c r="R21">
-        <v>0.73</v>
+        <v>5.77</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
@@ -5809,55 +5818,55 @@
         <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D22" s="12">
-        <v>2116</v>
+        <v>8325</v>
       </c>
       <c r="E22" s="12">
-        <v>2081</v>
+        <v>8170</v>
       </c>
       <c r="F22" s="13">
-        <v>0.98350000000000004</v>
+        <v>0.98140000000000005</v>
       </c>
       <c r="G22">
-        <v>35</v>
+        <v>155</v>
       </c>
       <c r="H22" s="13">
-        <v>1.6500000000000001E-2</v>
+        <v>1.8599999999999998E-2</v>
       </c>
       <c r="I22" s="12">
-        <v>1944</v>
+        <v>7649</v>
       </c>
       <c r="J22">
-        <v>73</v>
+        <v>233</v>
       </c>
       <c r="K22">
-        <v>64</v>
+        <v>288</v>
       </c>
       <c r="L22">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="M22">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="N22">
         <v>0</v>
       </c>
       <c r="O22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P22">
-        <v>0.76</v>
+        <v>0.73</v>
       </c>
       <c r="Q22">
-        <v>2.78</v>
+        <v>3.51</v>
       </c>
       <c r="R22">
-        <v>5.27</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
@@ -5865,40 +5874,40 @@
         <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="D23" s="12">
-        <v>1515</v>
+        <v>2159</v>
       </c>
       <c r="E23" s="12">
-        <v>1506</v>
+        <v>1924</v>
       </c>
       <c r="F23" s="13">
-        <v>0.99409999999999998</v>
+        <v>0.89119999999999999</v>
       </c>
       <c r="G23">
-        <v>9</v>
+        <v>235</v>
       </c>
       <c r="H23" s="13">
-        <v>5.8999999999999999E-3</v>
+        <v>0.10879999999999999</v>
       </c>
       <c r="I23" s="12">
-        <v>1430</v>
+        <v>1651</v>
       </c>
       <c r="J23">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="K23">
-        <v>35</v>
+        <v>173</v>
       </c>
       <c r="L23">
-        <v>9</v>
+        <v>221</v>
       </c>
       <c r="M23">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -5907,13 +5916,13 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <v>1.1499999999999999</v>
+        <v>13.62</v>
       </c>
       <c r="Q23">
-        <v>10.6</v>
+        <v>8.2100000000000009</v>
       </c>
       <c r="R23">
-        <v>1.27</v>
+        <v>1.63</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
@@ -5921,37 +5930,37 @@
         <v>73</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
-      </c>
-      <c r="D24">
-        <v>587</v>
-      </c>
-      <c r="E24">
-        <v>587</v>
+        <v>91</v>
+      </c>
+      <c r="D24" s="12">
+        <v>2464</v>
+      </c>
+      <c r="E24" s="12">
+        <v>2453</v>
       </c>
       <c r="F24" s="13">
-        <v>1</v>
+        <v>0.99550000000000005</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H24" s="13">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>584</v>
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="I24" s="12">
+        <v>2337</v>
       </c>
       <c r="J24">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -5960,66 +5969,72 @@
         <v>0</v>
       </c>
       <c r="O24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>1.25</v>
+      </c>
+      <c r="Q24">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="R24">
+        <v>2.16</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B25">
-        <v>-691</v>
+      <c r="B25" t="s">
+        <v>94</v>
       </c>
       <c r="C25" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D25" s="12">
-        <v>29437</v>
+        <v>1931</v>
       </c>
       <c r="E25" s="12">
-        <v>27487</v>
+        <v>1862</v>
       </c>
       <c r="F25" s="13">
-        <v>0.93379999999999996</v>
-      </c>
-      <c r="G25" s="12">
-        <v>1950</v>
+        <v>0.96430000000000005</v>
+      </c>
+      <c r="G25">
+        <v>69</v>
       </c>
       <c r="H25" s="13">
-        <v>6.6199999999999995E-2</v>
+        <v>3.5700000000000003E-2</v>
       </c>
       <c r="I25" s="12">
-        <v>23783</v>
-      </c>
-      <c r="J25" s="12">
-        <v>1612</v>
-      </c>
-      <c r="K25" s="12">
-        <v>2092</v>
-      </c>
-      <c r="L25" s="12">
-        <v>1590</v>
+        <v>1627</v>
+      </c>
+      <c r="J25">
+        <v>124</v>
+      </c>
+      <c r="K25">
+        <v>111</v>
+      </c>
+      <c r="L25">
+        <v>54</v>
       </c>
       <c r="M25">
-        <v>244</v>
+        <v>8</v>
       </c>
       <c r="N25">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="O25">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="P25">
-        <v>4.12</v>
+        <v>5.49</v>
       </c>
       <c r="Q25">
-        <v>8.81</v>
+        <v>6.71</v>
       </c>
       <c r="R25">
-        <v>2.25</v>
+        <v>7.21</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
@@ -6027,167 +6042,161 @@
         <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
-      </c>
-      <c r="D26" s="12">
-        <v>15273</v>
-      </c>
-      <c r="E26" s="12">
-        <v>14067</v>
+        <v>111</v>
+      </c>
+      <c r="D26">
+        <v>587</v>
+      </c>
+      <c r="E26">
+        <v>587</v>
       </c>
       <c r="F26" s="13">
-        <v>0.92100000000000004</v>
-      </c>
-      <c r="G26" s="12">
-        <v>1206</v>
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
       </c>
       <c r="H26" s="13">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="I26" s="12">
-        <v>11852</v>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>584</v>
       </c>
       <c r="J26">
-        <v>890</v>
-      </c>
-      <c r="K26" s="12">
-        <v>1325</v>
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
       </c>
       <c r="L26">
-        <v>815</v>
+        <v>0</v>
       </c>
       <c r="M26">
-        <v>267</v>
+        <v>0</v>
       </c>
       <c r="N26">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="O26">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="P26">
-        <v>3.76</v>
-      </c>
-      <c r="Q26">
-        <v>10.77</v>
-      </c>
-      <c r="R26">
-        <v>10.09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B27" t="s">
-        <v>115</v>
+      <c r="B27">
+        <v>-664</v>
       </c>
       <c r="C27" t="s">
-        <v>116</v>
-      </c>
-      <c r="D27">
-        <v>869</v>
-      </c>
-      <c r="E27">
-        <v>865</v>
+        <v>98</v>
+      </c>
+      <c r="D27" s="12">
+        <v>35352</v>
+      </c>
+      <c r="E27" s="12">
+        <v>34542</v>
       </c>
       <c r="F27" s="13">
-        <v>0.99539999999999995</v>
+        <v>0.97709999999999997</v>
       </c>
       <c r="G27">
-        <v>4</v>
+        <v>810</v>
       </c>
       <c r="H27" s="13">
-        <v>4.5999999999999999E-3</v>
-      </c>
-      <c r="I27">
-        <v>794</v>
+        <v>2.29E-2</v>
+      </c>
+      <c r="I27" s="12">
+        <v>32679</v>
       </c>
       <c r="J27">
-        <v>44</v>
-      </c>
-      <c r="K27">
-        <v>27</v>
+        <v>815</v>
+      </c>
+      <c r="K27" s="12">
+        <v>1048</v>
       </c>
       <c r="L27">
-        <v>3</v>
+        <v>557</v>
       </c>
       <c r="M27">
-        <v>0</v>
+        <v>184</v>
       </c>
       <c r="N27">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="O27">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="P27">
-        <v>1.97</v>
+        <v>0.63</v>
       </c>
       <c r="Q27">
-        <v>4.74</v>
+        <v>3.84</v>
       </c>
       <c r="R27">
-        <v>1.33</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
+      <c r="A28" t="s">
         <v>73</v>
       </c>
-      <c r="B28" t="s">
-        <v>117</v>
-      </c>
-      <c r="C28" t="s">
-        <v>118</v>
-      </c>
-      <c r="D28">
-        <v>716</v>
-      </c>
-      <c r="E28">
-        <v>716</v>
+      <c r="B28">
+        <v>-664</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" s="12">
+        <v>59606</v>
+      </c>
+      <c r="E28" s="12">
+        <v>58373</v>
       </c>
       <c r="F28" s="13">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
+        <v>0.97929999999999995</v>
+      </c>
+      <c r="G28" s="12">
+        <v>1233</v>
       </c>
       <c r="H28" s="13">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>709</v>
-      </c>
-      <c r="J28">
-        <v>2</v>
-      </c>
-      <c r="K28">
-        <v>5</v>
+        <v>2.07E-2</v>
+      </c>
+      <c r="I28" s="12">
+        <v>54522</v>
+      </c>
+      <c r="J28" s="12">
+        <v>1643</v>
+      </c>
+      <c r="K28" s="12">
+        <v>2208</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>931</v>
       </c>
       <c r="M28">
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="N28">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="O28">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P28">
-        <v>0.31</v>
+        <v>0.84</v>
       </c>
       <c r="Q28">
-        <v>0.06</v>
+        <v>4.04</v>
       </c>
       <c r="R28">
-        <v>0.03</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
@@ -6195,55 +6204,46 @@
         <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
-      </c>
-      <c r="C29" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29" s="12">
-        <v>3799</v>
-      </c>
-      <c r="E29" s="12">
-        <v>3748</v>
+        <v>99</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29">
+        <v>66</v>
+      </c>
+      <c r="E29">
+        <v>66</v>
       </c>
       <c r="F29" s="13">
-        <v>0.98660000000000003</v>
+        <v>1</v>
       </c>
       <c r="G29">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="H29" s="13">
-        <v>1.34E-2</v>
-      </c>
-      <c r="I29" s="12">
-        <v>3292</v>
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>66</v>
       </c>
       <c r="J29">
-        <v>290</v>
+        <v>0</v>
       </c>
       <c r="K29">
-        <v>166</v>
+        <v>0</v>
       </c>
       <c r="L29">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="M29">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="N29">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O29">
-        <v>3</v>
-      </c>
-      <c r="P29">
-        <v>3.58</v>
-      </c>
-      <c r="Q29">
-        <v>3.27</v>
-      </c>
-      <c r="R29">
-        <v>4.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
@@ -6251,55 +6251,55 @@
         <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C30" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D30" s="12">
-        <v>8106</v>
+        <v>1276</v>
       </c>
       <c r="E30" s="12">
-        <v>7751</v>
+        <v>1244</v>
       </c>
       <c r="F30" s="13">
-        <v>0.95620000000000005</v>
+        <v>0.97489999999999999</v>
       </c>
       <c r="G30">
-        <v>355</v>
+        <v>32</v>
       </c>
       <c r="H30" s="13">
-        <v>4.3799999999999999E-2</v>
+        <v>2.5100000000000001E-2</v>
       </c>
       <c r="I30" s="12">
-        <v>6947</v>
+        <v>1076</v>
       </c>
       <c r="J30">
-        <v>340</v>
+        <v>99</v>
       </c>
       <c r="K30">
-        <v>464</v>
+        <v>69</v>
       </c>
       <c r="L30">
-        <v>305</v>
+        <v>15</v>
       </c>
       <c r="M30">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="N30">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P30">
-        <v>5.21</v>
+        <v>2.59</v>
       </c>
       <c r="Q30">
-        <v>5.04</v>
+        <v>7.74</v>
       </c>
       <c r="R30">
-        <v>7.45</v>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
@@ -6307,55 +6307,55 @@
         <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>123</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
-      </c>
-      <c r="D31">
-        <v>955</v>
-      </c>
-      <c r="E31">
-        <v>944</v>
+        <v>77</v>
+      </c>
+      <c r="D31" s="12">
+        <v>3105</v>
+      </c>
+      <c r="E31" s="12">
+        <v>2949</v>
       </c>
       <c r="F31" s="13">
-        <v>0.98850000000000005</v>
+        <v>0.94979999999999998</v>
       </c>
       <c r="G31">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="H31" s="13">
-        <v>1.15E-2</v>
-      </c>
-      <c r="I31">
-        <v>929</v>
+        <v>5.0200000000000002E-2</v>
+      </c>
+      <c r="I31" s="12">
+        <v>2585</v>
       </c>
       <c r="J31">
-        <v>3</v>
+        <v>153</v>
       </c>
       <c r="K31">
-        <v>12</v>
+        <v>211</v>
       </c>
       <c r="L31">
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="M31">
+        <v>14</v>
+      </c>
+      <c r="N31">
         <v>2</v>
       </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
       <c r="O31">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P31">
-        <v>0.64</v>
+        <v>7.55</v>
       </c>
       <c r="Q31">
-        <v>15</v>
+        <v>10.36</v>
       </c>
       <c r="R31">
-        <v>1.81</v>
+        <v>4.87</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
@@ -6363,55 +6363,55 @@
         <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
-      </c>
-      <c r="D32" s="12">
-        <v>1047</v>
+        <v>116</v>
+      </c>
+      <c r="D32">
+        <v>869</v>
       </c>
       <c r="E32">
-        <v>946</v>
+        <v>865</v>
       </c>
       <c r="F32" s="13">
-        <v>0.90349999999999997</v>
+        <v>0.99539999999999995</v>
       </c>
       <c r="G32">
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="H32" s="13">
-        <v>9.6500000000000002E-2</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="I32">
-        <v>786</v>
+        <v>794</v>
       </c>
       <c r="J32">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="K32">
-        <v>97</v>
+        <v>27</v>
       </c>
       <c r="L32">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="M32">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O32">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P32">
-        <v>10.11</v>
+        <v>1.97</v>
       </c>
       <c r="Q32">
-        <v>11.31</v>
+        <v>4.74</v>
       </c>
       <c r="R32">
-        <v>0.04</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
@@ -6419,55 +6419,55 @@
         <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>127</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>128</v>
+        <v>81</v>
       </c>
       <c r="D33" s="12">
-        <v>1276</v>
+        <v>1218</v>
       </c>
       <c r="E33" s="12">
-        <v>1244</v>
+        <v>1199</v>
       </c>
       <c r="F33" s="13">
-        <v>0.97489999999999999</v>
+        <v>0.98440000000000005</v>
       </c>
       <c r="G33">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="H33" s="13">
-        <v>2.5100000000000001E-2</v>
+        <v>1.5599999999999999E-2</v>
       </c>
       <c r="I33" s="12">
-        <v>1076</v>
+        <v>1052</v>
       </c>
       <c r="J33">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K33">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="L33">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N33">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="O33">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P33">
-        <v>2.59</v>
+        <v>4.12</v>
       </c>
       <c r="Q33">
-        <v>7.74</v>
+        <v>12.92</v>
       </c>
       <c r="R33">
-        <v>9.6999999999999993</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
@@ -6531,170 +6531,173 @@
         <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="D35" s="12">
-        <v>2159</v>
+        <v>15273</v>
       </c>
       <c r="E35" s="12">
-        <v>1924</v>
+        <v>14067</v>
       </c>
       <c r="F35" s="13">
-        <v>0.89119999999999999</v>
-      </c>
-      <c r="G35">
-        <v>235</v>
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="G35" s="12">
+        <v>1206</v>
       </c>
       <c r="H35" s="13">
-        <v>0.10879999999999999</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="I35" s="12">
-        <v>1651</v>
+        <v>11852</v>
       </c>
       <c r="J35">
-        <v>100</v>
-      </c>
-      <c r="K35">
-        <v>173</v>
+        <v>890</v>
+      </c>
+      <c r="K35" s="12">
+        <v>1325</v>
       </c>
       <c r="L35">
-        <v>221</v>
+        <v>815</v>
       </c>
       <c r="M35">
-        <v>14</v>
+        <v>267</v>
       </c>
       <c r="N35">
+        <v>82</v>
+      </c>
+      <c r="O35">
+        <v>42</v>
+      </c>
+      <c r="P35">
+        <v>3.76</v>
+      </c>
+      <c r="Q35">
+        <v>10.77</v>
+      </c>
+      <c r="R35">
+        <v>10.09</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="12">
+        <v>1582</v>
+      </c>
+      <c r="E36" s="12">
+        <v>1558</v>
+      </c>
+      <c r="F36" s="13">
+        <v>0.98480000000000001</v>
+      </c>
+      <c r="G36">
+        <v>24</v>
+      </c>
+      <c r="H36" s="13">
+        <v>1.52E-2</v>
+      </c>
+      <c r="I36" s="12">
+        <v>1415</v>
+      </c>
+      <c r="J36">
+        <v>56</v>
+      </c>
+      <c r="K36">
+        <v>87</v>
+      </c>
+      <c r="L36">
+        <v>21</v>
+      </c>
+      <c r="M36">
+        <v>2</v>
+      </c>
+      <c r="N36">
         <v>0</v>
       </c>
-      <c r="O35">
-        <v>0</v>
-      </c>
-      <c r="P35">
-        <v>13.62</v>
-      </c>
-      <c r="Q35">
-        <v>8.2100000000000009</v>
-      </c>
-      <c r="R35">
-        <v>1.63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <v>0.51</v>
+      </c>
+      <c r="Q36">
+        <v>4</v>
+      </c>
+      <c r="R36">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>-691</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="D36" s="12">
-        <v>66418</v>
-      </c>
-      <c r="E36" s="12">
-        <v>62380</v>
-      </c>
-      <c r="F36" s="13">
-        <v>0.93920000000000003</v>
-      </c>
-      <c r="G36" s="12">
-        <v>4038</v>
-      </c>
-      <c r="H36" s="13">
-        <v>6.08E-2</v>
-      </c>
-      <c r="I36" s="12">
-        <v>54042</v>
-      </c>
-      <c r="J36" s="12">
-        <v>3717</v>
-      </c>
-      <c r="K36" s="12">
-        <v>4621</v>
-      </c>
-      <c r="L36" s="12">
-        <v>3141</v>
-      </c>
-      <c r="M36">
-        <v>605</v>
-      </c>
-      <c r="N36">
-        <v>181</v>
-      </c>
-      <c r="O36">
-        <v>111</v>
-      </c>
-      <c r="P36">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="Q36">
-        <v>8.7200000000000006</v>
-      </c>
-      <c r="R36">
-        <v>4.6900000000000004</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37">
-        <v>-664</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>138</v>
+      <c r="C37" t="s">
+        <v>112</v>
       </c>
       <c r="D37" s="12">
-        <v>59606</v>
+        <v>29437</v>
       </c>
       <c r="E37" s="12">
-        <v>58373</v>
+        <v>27487</v>
       </c>
       <c r="F37" s="13">
-        <v>0.97929999999999995</v>
+        <v>0.93379999999999996</v>
       </c>
       <c r="G37" s="12">
-        <v>1233</v>
+        <v>1950</v>
       </c>
       <c r="H37" s="13">
-        <v>2.07E-2</v>
+        <v>6.6199999999999995E-2</v>
       </c>
       <c r="I37" s="12">
-        <v>54522</v>
+        <v>23783</v>
       </c>
       <c r="J37" s="12">
-        <v>1643</v>
+        <v>1612</v>
       </c>
       <c r="K37" s="12">
-        <v>2208</v>
-      </c>
-      <c r="L37">
-        <v>931</v>
+        <v>2092</v>
+      </c>
+      <c r="L37" s="12">
+        <v>1590</v>
       </c>
       <c r="M37">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="N37">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O37">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="P37">
-        <v>0.84</v>
+        <v>4.12</v>
       </c>
       <c r="Q37">
-        <v>4.04</v>
+        <v>8.81</v>
       </c>
       <c r="R37">
-        <v>2.68</v>
+        <v>2.25</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R37">
+    <sortCondition ref="C2:C37"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added VA medical Center data from Long Beach and Loma linda
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Takano_fellowship/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E94C05-38BD-3743-AC30-A93459F4ED83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE4EACE-3883-BA4C-8347-8AD6E7341A69}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="560" windowWidth="25300" windowHeight="16020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="460" windowWidth="25300" windowHeight="15960" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sources" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,26 @@
     <sheet name="Census_riverside" sheetId="3" r:id="rId3"/>
     <sheet name="Vet_census" sheetId="4" r:id="rId4"/>
     <sheet name="VA_waittimes" sheetId="5" r:id="rId5"/>
+    <sheet name="LomaLinda_rating_va" sheetId="6" r:id="rId6"/>
+    <sheet name="LongBeach_rating_va" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mhNyi2lPXx3a1vk3up84biCzYKPjQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mhNyi2lPXx3a1vk3up84biCzYKPjQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="216">
   <si>
     <t>https://www.fbo.gov/index.php?s=opportunity&amp;mode=form&amp;id=18bf7ffdbb68421c11268ebf27cc86cd&amp;tab=core&amp;tabmode=list&amp;=</t>
   </si>
@@ -497,13 +505,193 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>VA Data Date Range</t>
+  </si>
+  <si>
+    <t>Is Higher or Lower Score Better?</t>
+  </si>
+  <si>
+    <t>Loma Linda VA Medical Center</t>
+  </si>
+  <si>
+    <t>Regional Average - Commercial</t>
+  </si>
+  <si>
+    <t>Regional Average - Medicaid</t>
+  </si>
+  <si>
+    <t>Regional Average - Medicare</t>
+  </si>
+  <si>
+    <t>National Average - Commercial</t>
+  </si>
+  <si>
+    <t>National Average - Medicaid</t>
+  </si>
+  <si>
+    <t>National Average - Medicare</t>
+  </si>
+  <si>
+    <t>Colorectal Cancer Screening</t>
+  </si>
+  <si>
+    <t>2017-10 - 2018-09</t>
+  </si>
+  <si>
+    <t>Higher is Better</t>
+  </si>
+  <si>
+    <t>Not Available</t>
+  </si>
+  <si>
+    <t>Flu Vaccinations for Adults Ages 18-64</t>
+  </si>
+  <si>
+    <t>Medical Assistance with Smoking and Tobacco Use Cessation - Advising Smokers To Quit</t>
+  </si>
+  <si>
+    <t>Medical Assistance with Smoking and Tobacco Use Cessation - Discussing Cessation Medications</t>
+  </si>
+  <si>
+    <t>Medical Assistance with Smoking and Tobacco Use Cessation - Discussing Cessation Strategies</t>
+  </si>
+  <si>
+    <t>Non-Recommended PSA-Based Screening in Older Men</t>
+  </si>
+  <si>
+    <t>Lower is Better</t>
+  </si>
+  <si>
+    <t>Breast Cancer Screening</t>
+  </si>
+  <si>
+    <t>Cervical Cancer Screening</t>
+  </si>
+  <si>
+    <t>Controlling High Blood Pressure</t>
+  </si>
+  <si>
+    <t>Persistence of Beta-Blocker Treatment after a Heart Attack</t>
+  </si>
+  <si>
+    <t>Statin Therapy for Patients With Cardiovascular Disease Received Statin Therapy - 21-75 years (Male)</t>
+  </si>
+  <si>
+    <t>Statin Therapy for Patients With Cardiovascular Disease Received Statin Therapy - 40-75 years (Female)</t>
+  </si>
+  <si>
+    <t>Statin Therapy for Patients With Cardiovascular Disease Received Statin Therapy - Total</t>
+  </si>
+  <si>
+    <t>Comprehensive Diabetes Care - Blood Pressure Control (&lt;140/90)</t>
+  </si>
+  <si>
+    <t>Comprehensive Diabetes Care - Eye Exams</t>
+  </si>
+  <si>
+    <t>Comprehensive Diabetes Care - HbA1c Control (&lt;7% for a selected population)</t>
+  </si>
+  <si>
+    <t>Comprehensive Diabetes Care - HbA1c Testing</t>
+  </si>
+  <si>
+    <t>Comprehensive Diabetes Care - Medical Attention for Nephropathy</t>
+  </si>
+  <si>
+    <t>Comprehensive Diabetes Care - Poor HbA1c Control</t>
+  </si>
+  <si>
+    <t>Statin Therapy for Patients With Diabetes Received Statin Therapy</t>
+  </si>
+  <si>
+    <t>Antidepressant Medication Management - Effective Acute Phase Treatment</t>
+  </si>
+  <si>
+    <t>Antidepressant Medication Management - Effective Continuation Phase Treatment</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>VA Long Beach Healthcare System</t>
+  </si>
+  <si>
+    <t>Facility</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>F13</t>
+  </si>
+  <si>
+    <t>F14</t>
+  </si>
+  <si>
+    <t>F15</t>
+  </si>
+  <si>
+    <t>F16</t>
+  </si>
+  <si>
+    <t>F17</t>
+  </si>
+  <si>
+    <t>F18</t>
+  </si>
+  <si>
+    <t>F19</t>
+  </si>
+  <si>
+    <t>F20</t>
+  </si>
+  <si>
+    <t>F21</t>
+  </si>
+  <si>
+    <t>F22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -547,6 +735,12 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -557,6 +751,29 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.8"/>
+      <color rgb="FF99CEF7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -576,10 +793,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -591,15 +809,22 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4636,11 +4861,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9669893B-6154-FA47-910F-11235E69FDD3}">
   <dimension ref="A1:AU37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:R37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="C1" s="10" t="s">
@@ -6700,4 +6929,1595 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FF8F07-5387-664E-989D-185CF4B0D514}">
+  <dimension ref="A1:W66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="18">
+        <v>75.62</v>
+      </c>
+      <c r="C2" s="18">
+        <v>44.26</v>
+      </c>
+      <c r="D2" s="18">
+        <v>97.23</v>
+      </c>
+      <c r="E2" s="18">
+        <v>95.88</v>
+      </c>
+      <c r="F2" s="18">
+        <v>97.24</v>
+      </c>
+      <c r="G2" s="18">
+        <v>19.739999999999998</v>
+      </c>
+      <c r="H2" s="18">
+        <v>81.73</v>
+      </c>
+      <c r="I2" s="18">
+        <v>80.92</v>
+      </c>
+      <c r="J2" s="18">
+        <v>76.66</v>
+      </c>
+      <c r="K2" s="18">
+        <v>92.37</v>
+      </c>
+      <c r="L2" s="18">
+        <v>78.14</v>
+      </c>
+      <c r="M2" s="18">
+        <v>70.12</v>
+      </c>
+      <c r="N2" s="18">
+        <v>78.02</v>
+      </c>
+      <c r="O2" s="18">
+        <v>77.459999999999994</v>
+      </c>
+      <c r="P2" s="18">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="Q2" s="18">
+        <v>38.93</v>
+      </c>
+      <c r="R2" s="18">
+        <v>98.21</v>
+      </c>
+      <c r="S2" s="18">
+        <v>98.02</v>
+      </c>
+      <c r="T2" s="18">
+        <v>27.37</v>
+      </c>
+      <c r="U2" s="18">
+        <v>69.680000000000007</v>
+      </c>
+      <c r="V2" s="18">
+        <v>68.37</v>
+      </c>
+      <c r="W2" s="18">
+        <v>54.23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="18">
+        <v>83.1</v>
+      </c>
+      <c r="C3" s="18">
+        <v>46.62</v>
+      </c>
+      <c r="D3" s="18">
+        <v>98.84</v>
+      </c>
+      <c r="E3" s="18">
+        <v>97.59</v>
+      </c>
+      <c r="F3" s="18">
+        <v>98.84</v>
+      </c>
+      <c r="G3" s="18">
+        <v>20.350000000000001</v>
+      </c>
+      <c r="H3" s="18">
+        <v>82.13</v>
+      </c>
+      <c r="I3" s="18">
+        <v>92.36</v>
+      </c>
+      <c r="J3" s="18">
+        <v>76.11</v>
+      </c>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18">
+        <v>84.61</v>
+      </c>
+      <c r="M3" s="18">
+        <v>81.44</v>
+      </c>
+      <c r="N3" s="18">
+        <v>84.56</v>
+      </c>
+      <c r="O3" s="18">
+        <v>69.790000000000006</v>
+      </c>
+      <c r="P3" s="18">
+        <v>91.68</v>
+      </c>
+      <c r="Q3" s="18">
+        <v>43.31</v>
+      </c>
+      <c r="R3" s="18">
+        <v>98.7</v>
+      </c>
+      <c r="S3" s="18">
+        <v>99.37</v>
+      </c>
+      <c r="T3" s="18">
+        <v>15</v>
+      </c>
+      <c r="U3" s="18">
+        <v>71.19</v>
+      </c>
+      <c r="V3" s="18">
+        <v>84.53</v>
+      </c>
+      <c r="W3" s="18">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="18">
+        <v>58.55</v>
+      </c>
+      <c r="C4" s="18">
+        <v>51.53</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18">
+        <v>69.86</v>
+      </c>
+      <c r="I4" s="18">
+        <v>71.489999999999995</v>
+      </c>
+      <c r="J4" s="18">
+        <v>53.96</v>
+      </c>
+      <c r="K4" s="18">
+        <v>80.540000000000006</v>
+      </c>
+      <c r="L4" s="18">
+        <v>81.239999999999995</v>
+      </c>
+      <c r="M4" s="18">
+        <v>70.08</v>
+      </c>
+      <c r="N4" s="18">
+        <v>78.03</v>
+      </c>
+      <c r="O4" s="18">
+        <v>59.38</v>
+      </c>
+      <c r="P4" s="18">
+        <v>48.67</v>
+      </c>
+      <c r="Q4" s="18">
+        <v>43.67</v>
+      </c>
+      <c r="R4" s="18">
+        <v>89.41</v>
+      </c>
+      <c r="S4" s="18">
+        <v>89.29</v>
+      </c>
+      <c r="T4" s="18">
+        <v>34.29</v>
+      </c>
+      <c r="U4" s="18">
+        <v>59.74</v>
+      </c>
+      <c r="V4" s="18">
+        <v>64.430000000000007</v>
+      </c>
+      <c r="W4" s="18">
+        <v>49.16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18">
+        <v>40.67</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18">
+        <v>57.28</v>
+      </c>
+      <c r="I5" s="18">
+        <v>59.78</v>
+      </c>
+      <c r="J5" s="18">
+        <v>63.65</v>
+      </c>
+      <c r="K5" s="18">
+        <v>76.28</v>
+      </c>
+      <c r="L5" s="18">
+        <v>77.72</v>
+      </c>
+      <c r="M5" s="18">
+        <v>69.38</v>
+      </c>
+      <c r="N5" s="18">
+        <v>74.47</v>
+      </c>
+      <c r="O5" s="18">
+        <v>67.83</v>
+      </c>
+      <c r="P5" s="18">
+        <v>60.72</v>
+      </c>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18">
+        <v>87.85</v>
+      </c>
+      <c r="S5" s="18">
+        <v>90.16</v>
+      </c>
+      <c r="T5" s="18">
+        <v>35.1</v>
+      </c>
+      <c r="U5" s="18">
+        <v>64.819999999999993</v>
+      </c>
+      <c r="V5" s="18">
+        <v>57.49</v>
+      </c>
+      <c r="W5" s="18">
+        <v>41.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="18">
+        <v>70.47</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18">
+        <v>32.25</v>
+      </c>
+      <c r="H6" s="18">
+        <v>71.97</v>
+      </c>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18">
+        <v>71.62</v>
+      </c>
+      <c r="K6" s="18">
+        <v>88.15</v>
+      </c>
+      <c r="L6" s="18">
+        <v>79.760000000000005</v>
+      </c>
+      <c r="M6" s="18">
+        <v>73.94</v>
+      </c>
+      <c r="N6" s="18">
+        <v>77.650000000000006</v>
+      </c>
+      <c r="O6" s="18">
+        <v>65.5</v>
+      </c>
+      <c r="P6" s="18">
+        <v>74.319999999999993</v>
+      </c>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18">
+        <v>94.37</v>
+      </c>
+      <c r="S6" s="18">
+        <v>96.43</v>
+      </c>
+      <c r="T6" s="18">
+        <v>21.58</v>
+      </c>
+      <c r="U6" s="18">
+        <v>72.03</v>
+      </c>
+      <c r="V6" s="18">
+        <v>69.459999999999994</v>
+      </c>
+      <c r="W6" s="18">
+        <v>53.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="18">
+        <v>61.05</v>
+      </c>
+      <c r="C7" s="18">
+        <v>50.02</v>
+      </c>
+      <c r="D7" s="18">
+        <v>74.52</v>
+      </c>
+      <c r="E7" s="18">
+        <v>50.4</v>
+      </c>
+      <c r="F7" s="18">
+        <v>44.37</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18">
+        <v>71.37</v>
+      </c>
+      <c r="I7" s="18">
+        <v>73.75</v>
+      </c>
+      <c r="J7" s="18">
+        <v>58.48</v>
+      </c>
+      <c r="K7" s="18">
+        <v>84.56</v>
+      </c>
+      <c r="L7" s="18">
+        <v>82.98</v>
+      </c>
+      <c r="M7" s="18">
+        <v>73.38</v>
+      </c>
+      <c r="N7" s="18">
+        <v>80.680000000000007</v>
+      </c>
+      <c r="O7" s="18">
+        <v>56.05</v>
+      </c>
+      <c r="P7" s="18">
+        <v>51.92</v>
+      </c>
+      <c r="Q7" s="18">
+        <v>37.9</v>
+      </c>
+      <c r="R7" s="18">
+        <v>90.49</v>
+      </c>
+      <c r="S7" s="18">
+        <v>89.25</v>
+      </c>
+      <c r="T7" s="18">
+        <v>36.44</v>
+      </c>
+      <c r="U7" s="18">
+        <v>60.76</v>
+      </c>
+      <c r="V7" s="18">
+        <v>67.989999999999995</v>
+      </c>
+      <c r="W7" s="18">
+        <v>52.38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18">
+        <v>39.6</v>
+      </c>
+      <c r="D8" s="18">
+        <v>76.97</v>
+      </c>
+      <c r="E8" s="18">
+        <v>51.53</v>
+      </c>
+      <c r="F8" s="18">
+        <v>45.37</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18">
+        <v>58.28</v>
+      </c>
+      <c r="I8" s="18">
+        <v>59.42</v>
+      </c>
+      <c r="J8" s="18">
+        <v>56.92</v>
+      </c>
+      <c r="K8" s="18">
+        <v>78.459999999999994</v>
+      </c>
+      <c r="L8" s="18">
+        <v>77.75</v>
+      </c>
+      <c r="M8" s="18">
+        <v>73.430000000000007</v>
+      </c>
+      <c r="N8" s="18">
+        <v>76.17</v>
+      </c>
+      <c r="O8" s="18">
+        <v>62.69</v>
+      </c>
+      <c r="P8" s="18">
+        <v>57.2</v>
+      </c>
+      <c r="Q8" s="18">
+        <v>34.590000000000003</v>
+      </c>
+      <c r="R8" s="18">
+        <v>87.54</v>
+      </c>
+      <c r="S8" s="18">
+        <v>90.11</v>
+      </c>
+      <c r="T8" s="18">
+        <v>40.520000000000003</v>
+      </c>
+      <c r="U8" s="18">
+        <v>61.46</v>
+      </c>
+      <c r="V8" s="18">
+        <v>53.9</v>
+      </c>
+      <c r="W8" s="18">
+        <v>38.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="18">
+        <v>70.040000000000006</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18">
+        <v>31.52</v>
+      </c>
+      <c r="H9" s="18">
+        <v>72.45</v>
+      </c>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18">
+        <v>71.14</v>
+      </c>
+      <c r="K9" s="18">
+        <v>90.15</v>
+      </c>
+      <c r="L9" s="18">
+        <v>80.38</v>
+      </c>
+      <c r="M9" s="18">
+        <v>76.849999999999994</v>
+      </c>
+      <c r="N9" s="18">
+        <v>79.010000000000005</v>
+      </c>
+      <c r="O9" s="18">
+        <v>66.56</v>
+      </c>
+      <c r="P9" s="18">
+        <v>71.78</v>
+      </c>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18">
+        <v>93.67</v>
+      </c>
+      <c r="S9" s="18">
+        <v>95.56</v>
+      </c>
+      <c r="T9" s="18">
+        <v>24.72</v>
+      </c>
+      <c r="U9" s="18">
+        <v>71.67</v>
+      </c>
+      <c r="V9" s="18">
+        <v>70.87</v>
+      </c>
+      <c r="W9" s="18">
+        <v>56.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="14"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="14"/>
+      <c r="B11" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="M11" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="N11" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="O11" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="P11" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q11" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="R11" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="S11" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="T11" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="U11" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="V11" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="W11" s="18" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="17"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="17"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="17"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="17"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="17"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="17"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="17"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="17"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="17"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="17"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="17"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="17"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="17"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="14"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="14"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="14"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="14"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="14"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="14"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="14"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="14"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="14"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="14"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="14"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="15"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="14"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="14"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="14"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="14"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="14"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="14"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="14"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="14"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="14"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="14"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="14"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="15"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="14"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="14"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="14"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="14"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="14"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="14"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="14"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="14"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="14"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="15"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="14"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="14"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="14"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="16"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="14"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CE46A3-26B0-7140-862D-2B9EB01EDE3E}">
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="18">
+        <v>83.1</v>
+      </c>
+      <c r="E2" s="18">
+        <v>58.55</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" s="18">
+        <v>70.47</v>
+      </c>
+      <c r="H2" s="18">
+        <v>61.05</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="J2" s="18">
+        <v>70.040000000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="18">
+        <v>46.62</v>
+      </c>
+      <c r="E3" s="18">
+        <v>51.53</v>
+      </c>
+      <c r="F3" s="18">
+        <v>40.67</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="H3" s="18">
+        <v>50.02</v>
+      </c>
+      <c r="I3" s="18">
+        <v>39.6</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="18">
+        <v>98.84</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="H4" s="18">
+        <v>74.52</v>
+      </c>
+      <c r="I4" s="18">
+        <v>76.97</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="18">
+        <v>97.59</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" s="18">
+        <v>50.4</v>
+      </c>
+      <c r="I5" s="18">
+        <v>51.53</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="18">
+        <v>98.84</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="H6" s="18">
+        <v>44.37</v>
+      </c>
+      <c r="I6" s="18">
+        <v>45.37</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="18">
+        <v>20.350000000000001</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" s="18">
+        <v>32.25</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="J7" s="18">
+        <v>31.52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" s="18">
+        <v>82.13</v>
+      </c>
+      <c r="E8" s="18">
+        <v>69.86</v>
+      </c>
+      <c r="F8" s="18">
+        <v>57.28</v>
+      </c>
+      <c r="G8" s="18">
+        <v>71.97</v>
+      </c>
+      <c r="H8" s="18">
+        <v>71.37</v>
+      </c>
+      <c r="I8" s="18">
+        <v>58.28</v>
+      </c>
+      <c r="J8" s="18">
+        <v>72.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" s="18">
+        <v>92.36</v>
+      </c>
+      <c r="E9" s="18">
+        <v>71.489999999999995</v>
+      </c>
+      <c r="F9" s="18">
+        <v>59.78</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="H9" s="18">
+        <v>73.75</v>
+      </c>
+      <c r="I9" s="18">
+        <v>59.42</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="18">
+        <v>76.11</v>
+      </c>
+      <c r="E10" s="18">
+        <v>53.96</v>
+      </c>
+      <c r="F10" s="18">
+        <v>63.65</v>
+      </c>
+      <c r="G10" s="18">
+        <v>71.62</v>
+      </c>
+      <c r="H10" s="18">
+        <v>58.48</v>
+      </c>
+      <c r="I10" s="18">
+        <v>56.92</v>
+      </c>
+      <c r="J10" s="18">
+        <v>71.14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="E11" s="18">
+        <v>80.540000000000006</v>
+      </c>
+      <c r="F11" s="18">
+        <v>76.28</v>
+      </c>
+      <c r="G11" s="18">
+        <v>88.15</v>
+      </c>
+      <c r="H11" s="18">
+        <v>84.56</v>
+      </c>
+      <c r="I11" s="18">
+        <v>78.459999999999994</v>
+      </c>
+      <c r="J11" s="18">
+        <v>90.15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="18">
+        <v>84.61</v>
+      </c>
+      <c r="E12" s="18">
+        <v>81.239999999999995</v>
+      </c>
+      <c r="F12" s="18">
+        <v>77.72</v>
+      </c>
+      <c r="G12" s="18">
+        <v>79.760000000000005</v>
+      </c>
+      <c r="H12" s="18">
+        <v>82.98</v>
+      </c>
+      <c r="I12" s="18">
+        <v>77.75</v>
+      </c>
+      <c r="J12" s="18">
+        <v>80.38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="18">
+        <v>81.44</v>
+      </c>
+      <c r="E13" s="18">
+        <v>70.08</v>
+      </c>
+      <c r="F13" s="18">
+        <v>69.38</v>
+      </c>
+      <c r="G13" s="18">
+        <v>73.94</v>
+      </c>
+      <c r="H13" s="18">
+        <v>73.38</v>
+      </c>
+      <c r="I13" s="18">
+        <v>73.430000000000007</v>
+      </c>
+      <c r="J13" s="18">
+        <v>76.849999999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="18">
+        <v>84.56</v>
+      </c>
+      <c r="E14" s="18">
+        <v>78.03</v>
+      </c>
+      <c r="F14" s="18">
+        <v>74.47</v>
+      </c>
+      <c r="G14" s="18">
+        <v>77.650000000000006</v>
+      </c>
+      <c r="H14" s="18">
+        <v>80.680000000000007</v>
+      </c>
+      <c r="I14" s="18">
+        <v>76.17</v>
+      </c>
+      <c r="J14" s="18">
+        <v>79.010000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D15" s="18">
+        <v>69.790000000000006</v>
+      </c>
+      <c r="E15" s="18">
+        <v>59.38</v>
+      </c>
+      <c r="F15" s="18">
+        <v>67.83</v>
+      </c>
+      <c r="G15" s="18">
+        <v>65.5</v>
+      </c>
+      <c r="H15" s="18">
+        <v>56.05</v>
+      </c>
+      <c r="I15" s="18">
+        <v>62.69</v>
+      </c>
+      <c r="J15" s="18">
+        <v>66.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" s="18">
+        <v>91.68</v>
+      </c>
+      <c r="E16" s="18">
+        <v>48.67</v>
+      </c>
+      <c r="F16" s="18">
+        <v>60.72</v>
+      </c>
+      <c r="G16" s="18">
+        <v>74.319999999999993</v>
+      </c>
+      <c r="H16" s="18">
+        <v>51.92</v>
+      </c>
+      <c r="I16" s="18">
+        <v>57.2</v>
+      </c>
+      <c r="J16" s="18">
+        <v>71.78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" s="18">
+        <v>43.31</v>
+      </c>
+      <c r="E17" s="18">
+        <v>43.67</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="H17" s="18">
+        <v>37.9</v>
+      </c>
+      <c r="I17" s="18">
+        <v>34.590000000000003</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D18" s="18">
+        <v>98.7</v>
+      </c>
+      <c r="E18" s="18">
+        <v>89.41</v>
+      </c>
+      <c r="F18" s="18">
+        <v>87.85</v>
+      </c>
+      <c r="G18" s="18">
+        <v>94.37</v>
+      </c>
+      <c r="H18" s="18">
+        <v>90.49</v>
+      </c>
+      <c r="I18" s="18">
+        <v>87.54</v>
+      </c>
+      <c r="J18" s="18">
+        <v>93.67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" s="18">
+        <v>99.37</v>
+      </c>
+      <c r="E19" s="18">
+        <v>89.29</v>
+      </c>
+      <c r="F19" s="18">
+        <v>90.16</v>
+      </c>
+      <c r="G19" s="18">
+        <v>96.43</v>
+      </c>
+      <c r="H19" s="18">
+        <v>89.25</v>
+      </c>
+      <c r="I19" s="18">
+        <v>90.11</v>
+      </c>
+      <c r="J19" s="18">
+        <v>95.56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D20" s="18">
+        <v>15</v>
+      </c>
+      <c r="E20" s="18">
+        <v>34.29</v>
+      </c>
+      <c r="F20" s="18">
+        <v>35.1</v>
+      </c>
+      <c r="G20" s="18">
+        <v>21.58</v>
+      </c>
+      <c r="H20" s="18">
+        <v>36.44</v>
+      </c>
+      <c r="I20" s="18">
+        <v>40.520000000000003</v>
+      </c>
+      <c r="J20" s="18">
+        <v>24.72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21" s="18">
+        <v>71.19</v>
+      </c>
+      <c r="E21" s="18">
+        <v>59.74</v>
+      </c>
+      <c r="F21" s="18">
+        <v>64.819999999999993</v>
+      </c>
+      <c r="G21" s="18">
+        <v>72.03</v>
+      </c>
+      <c r="H21" s="18">
+        <v>60.76</v>
+      </c>
+      <c r="I21" s="18">
+        <v>61.46</v>
+      </c>
+      <c r="J21" s="18">
+        <v>71.67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" s="18">
+        <v>84.53</v>
+      </c>
+      <c r="E22" s="18">
+        <v>64.430000000000007</v>
+      </c>
+      <c r="F22" s="18">
+        <v>57.49</v>
+      </c>
+      <c r="G22" s="18">
+        <v>69.459999999999994</v>
+      </c>
+      <c r="H22" s="18">
+        <v>67.989999999999995</v>
+      </c>
+      <c r="I22" s="18">
+        <v>53.9</v>
+      </c>
+      <c r="J22" s="18">
+        <v>70.87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D23" s="18">
+        <v>68</v>
+      </c>
+      <c r="E23" s="18">
+        <v>49.16</v>
+      </c>
+      <c r="F23" s="18">
+        <v>41.03</v>
+      </c>
+      <c r="G23" s="18">
+        <v>53.25</v>
+      </c>
+      <c r="H23" s="18">
+        <v>52.38</v>
+      </c>
+      <c r="I23" s="18">
+        <v>38.6</v>
+      </c>
+      <c r="J23" s="18">
+        <v>56.06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>